<commit_message>
fixato copertura progettazione l'acceso ai test case per llm
</commit_message>
<xml_diff>
--- a/input/generated_test_cases3_label_rimosse_feedbackAI_testcase_progettazione.xlsx
+++ b/input/generated_test_cases3_label_rimosse_feedbackAI_testcase_progettazione.xlsx
@@ -10509,1419 +10509,2419 @@
       </c>
     </row>
     <row r="222">
-      <c r="R222" t="n">
+      <c r="A222" s="2" t="n"/>
+      <c r="B222" s="2" t="n"/>
+      <c r="C222" s="2" t="n"/>
+      <c r="D222" s="2" t="n"/>
+      <c r="E222" s="2" t="n"/>
+      <c r="F222" s="2" t="n"/>
+      <c r="G222" s="2" t="n"/>
+      <c r="H222" s="2" t="n"/>
+      <c r="I222" s="2" t="n"/>
+      <c r="J222" s="2" t="n"/>
+      <c r="K222" s="2" t="n"/>
+      <c r="L222" s="2" t="n"/>
+      <c r="M222" s="2" t="n"/>
+      <c r="N222" s="2" t="n"/>
+      <c r="O222" s="2" t="n"/>
+      <c r="P222" s="2" t="n"/>
+      <c r="Q222" s="2" t="n"/>
+      <c r="R222" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S222" t="inlineStr">
+      <c r="S222" s="2" t="inlineStr">
         <is>
           <t>For each pronostico, verify that the description is displayed as two strings: Stringa 1 (top, bold) and Stringa 2 (below, grey).</t>
         </is>
       </c>
-      <c r="T222" t="inlineStr">
+      <c r="T222" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in Italian, as per business mapping.</t>
         </is>
       </c>
+      <c r="U222" s="2" t="n"/>
+      <c r="V222" s="2" t="n"/>
+      <c r="W222" s="2" t="n"/>
+      <c r="X222" s="2" t="n"/>
+      <c r="Y222" s="2" t="n"/>
+      <c r="Z222" s="2" t="n"/>
+      <c r="AA222" s="2" t="n"/>
+      <c r="AB222" s="2" t="n"/>
+      <c r="AC222" s="2" t="n"/>
+      <c r="AD222" s="2" t="n"/>
+      <c r="AE222" s="2" t="n"/>
+      <c r="AF222" s="2" t="n"/>
+      <c r="AG222" s="2" t="n"/>
+      <c r="AH222" s="2" t="n"/>
+      <c r="AI222" s="2" t="n"/>
+      <c r="AJ222" s="2" t="n"/>
+      <c r="AK222" s="2" t="n"/>
     </row>
     <row r="223">
-      <c r="R223" t="n">
+      <c r="A223" s="2" t="n"/>
+      <c r="B223" s="2" t="n"/>
+      <c r="C223" s="2" t="n"/>
+      <c r="D223" s="2" t="n"/>
+      <c r="E223" s="2" t="n"/>
+      <c r="F223" s="2" t="n"/>
+      <c r="G223" s="2" t="n"/>
+      <c r="H223" s="2" t="n"/>
+      <c r="I223" s="2" t="n"/>
+      <c r="J223" s="2" t="n"/>
+      <c r="K223" s="2" t="n"/>
+      <c r="L223" s="2" t="n"/>
+      <c r="M223" s="2" t="n"/>
+      <c r="N223" s="2" t="n"/>
+      <c r="O223" s="2" t="n"/>
+      <c r="P223" s="2" t="n"/>
+      <c r="Q223" s="2" t="n"/>
+      <c r="R223" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="S223" t="inlineStr">
+      <c r="S223" s="2" t="inlineStr">
         <is>
           <t>Check that the descriptions are in Italian, as per the business mapping.</t>
         </is>
       </c>
-      <c r="T223" t="inlineStr">
+      <c r="T223" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in Italian, as per business mapping.</t>
         </is>
       </c>
+      <c r="U223" s="2" t="n"/>
+      <c r="V223" s="2" t="n"/>
+      <c r="W223" s="2" t="n"/>
+      <c r="X223" s="2" t="n"/>
+      <c r="Y223" s="2" t="n"/>
+      <c r="Z223" s="2" t="n"/>
+      <c r="AA223" s="2" t="n"/>
+      <c r="AB223" s="2" t="n"/>
+      <c r="AC223" s="2" t="n"/>
+      <c r="AD223" s="2" t="n"/>
+      <c r="AE223" s="2" t="n"/>
+      <c r="AF223" s="2" t="n"/>
+      <c r="AG223" s="2" t="n"/>
+      <c r="AH223" s="2" t="n"/>
+      <c r="AI223" s="2" t="n"/>
+      <c r="AJ223" s="2" t="n"/>
+      <c r="AK223" s="2" t="n"/>
     </row>
     <row r="224">
-      <c r="A224" t="inlineStr">
+      <c r="A224" s="2" t="inlineStr">
         <is>
           <t>Verify Pronostico Description Rendering in French (Full Responsive Marocco)</t>
         </is>
       </c>
-      <c r="C224" t="n">
+      <c r="B224" s="2" t="n"/>
+      <c r="C224" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="D224" t="inlineStr">
+      <c r="D224" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E224" t="inlineStr">
+      <c r="E224" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F224" t="inlineStr">
+      <c r="F224" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G224" t="inlineStr">
+      <c r="G224" s="2" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="H224" t="inlineStr">
+      <c r="H224" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I224" t="inlineStr">
+      <c r="I224" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web (Full Responsive Marocco)</t>
         </is>
       </c>
-      <c r="J224" t="inlineStr">
+      <c r="J224" s="2" t="inlineStr">
         <is>
           <t>SGP Generator has provided at least one precompilata with pronostici for the avvenimento. User is on the Full Responsive Marocco frontend.</t>
         </is>
       </c>
-      <c r="K224" t="inlineStr">
+      <c r="K224" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L224" t="inlineStr">
+      <c r="L224" s="2" t="inlineStr">
         <is>
           <t>Pronostico Description Rendering</t>
         </is>
       </c>
-      <c r="M224" t="inlineStr">
+      <c r="M224" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N224" t="n">
-        <v>1</v>
-      </c>
-      <c r="O224" t="n">
-        <v>1</v>
-      </c>
-      <c r="P224" t="inlineStr">
+      <c r="N224" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O224" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P224" s="2" t="inlineStr">
         <is>
           <t>Precompilata data with mapped French pronostici.</t>
         </is>
       </c>
-      <c r="R224" t="n">
-        <v>1</v>
-      </c>
-      <c r="S224" t="inlineStr">
+      <c r="Q224" s="2" t="n"/>
+      <c r="R224" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S224" s="2" t="inlineStr">
         <is>
           <t>Access the Carosello Dett Avv page on the Full Responsive Marocco frontend.</t>
         </is>
       </c>
-      <c r="T224" t="inlineStr">
+      <c r="T224" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in French, as per business mapping.</t>
         </is>
       </c>
-      <c r="U224" t="inlineStr">
+      <c r="U224" s="2" t="inlineStr">
         <is>
           <t>Morocco</t>
         </is>
       </c>
-      <c r="Y224" t="inlineStr">
+      <c r="V224" s="2" t="n"/>
+      <c r="W224" s="2" t="n"/>
+      <c r="X224" s="2" t="n"/>
+      <c r="Y224" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z224" t="inlineStr">
+      <c r="Z224" s="2" t="inlineStr">
         <is>
           <t>Covers cross-device/browser consistency for carousel skeleton.</t>
         </is>
       </c>
-      <c r="AA224" t="inlineStr">
+      <c r="AA224" s="2" t="inlineStr">
         <is>
           <t>Carosello Dett Avv – Struttura Card Precompilata</t>
         </is>
       </c>
+      <c r="AB224" s="2" t="n"/>
+      <c r="AC224" s="2" t="n"/>
+      <c r="AD224" s="2" t="n"/>
+      <c r="AE224" s="2" t="n"/>
+      <c r="AF224" s="2" t="n"/>
+      <c r="AG224" s="2" t="n"/>
+      <c r="AH224" s="2" t="n"/>
+      <c r="AI224" s="2" t="n"/>
+      <c r="AJ224" s="2" t="n"/>
+      <c r="AK224" s="2" t="n"/>
     </row>
     <row r="225">
-      <c r="R225" t="n">
+      <c r="A225" s="2" t="n"/>
+      <c r="B225" s="2" t="n"/>
+      <c r="C225" s="2" t="n"/>
+      <c r="D225" s="2" t="n"/>
+      <c r="E225" s="2" t="n"/>
+      <c r="F225" s="2" t="n"/>
+      <c r="G225" s="2" t="n"/>
+      <c r="H225" s="2" t="n"/>
+      <c r="I225" s="2" t="n"/>
+      <c r="J225" s="2" t="n"/>
+      <c r="K225" s="2" t="n"/>
+      <c r="L225" s="2" t="n"/>
+      <c r="M225" s="2" t="n"/>
+      <c r="N225" s="2" t="n"/>
+      <c r="O225" s="2" t="n"/>
+      <c r="P225" s="2" t="n"/>
+      <c r="Q225" s="2" t="n"/>
+      <c r="R225" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S225" t="inlineStr">
+      <c r="S225" s="2" t="inlineStr">
         <is>
           <t>Identify a precompilata card for a specific avvenimento.</t>
         </is>
       </c>
-      <c r="T225" t="inlineStr">
+      <c r="T225" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in French, as per business mapping.</t>
         </is>
       </c>
+      <c r="U225" s="2" t="n"/>
+      <c r="V225" s="2" t="n"/>
+      <c r="W225" s="2" t="n"/>
+      <c r="X225" s="2" t="n"/>
+      <c r="Y225" s="2" t="n"/>
+      <c r="Z225" s="2" t="n"/>
+      <c r="AA225" s="2" t="n"/>
+      <c r="AB225" s="2" t="n"/>
+      <c r="AC225" s="2" t="n"/>
+      <c r="AD225" s="2" t="n"/>
+      <c r="AE225" s="2" t="n"/>
+      <c r="AF225" s="2" t="n"/>
+      <c r="AG225" s="2" t="n"/>
+      <c r="AH225" s="2" t="n"/>
+      <c r="AI225" s="2" t="n"/>
+      <c r="AJ225" s="2" t="n"/>
+      <c r="AK225" s="2" t="n"/>
     </row>
     <row r="226">
-      <c r="R226" t="n">
+      <c r="A226" s="2" t="n"/>
+      <c r="B226" s="2" t="n"/>
+      <c r="C226" s="2" t="n"/>
+      <c r="D226" s="2" t="n"/>
+      <c r="E226" s="2" t="n"/>
+      <c r="F226" s="2" t="n"/>
+      <c r="G226" s="2" t="n"/>
+      <c r="H226" s="2" t="n"/>
+      <c r="I226" s="2" t="n"/>
+      <c r="J226" s="2" t="n"/>
+      <c r="K226" s="2" t="n"/>
+      <c r="L226" s="2" t="n"/>
+      <c r="M226" s="2" t="n"/>
+      <c r="N226" s="2" t="n"/>
+      <c r="O226" s="2" t="n"/>
+      <c r="P226" s="2" t="n"/>
+      <c r="Q226" s="2" t="n"/>
+      <c r="R226" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S226" t="inlineStr">
+      <c r="S226" s="2" t="inlineStr">
         <is>
           <t>For each pronostico, verify that the description is displayed as two strings: Stringa 1 (top, bold) and Stringa 2 (below, grey).</t>
         </is>
       </c>
-      <c r="T226" t="inlineStr">
+      <c r="T226" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in French, as per business mapping.</t>
         </is>
       </c>
+      <c r="U226" s="2" t="n"/>
+      <c r="V226" s="2" t="n"/>
+      <c r="W226" s="2" t="n"/>
+      <c r="X226" s="2" t="n"/>
+      <c r="Y226" s="2" t="n"/>
+      <c r="Z226" s="2" t="n"/>
+      <c r="AA226" s="2" t="n"/>
+      <c r="AB226" s="2" t="n"/>
+      <c r="AC226" s="2" t="n"/>
+      <c r="AD226" s="2" t="n"/>
+      <c r="AE226" s="2" t="n"/>
+      <c r="AF226" s="2" t="n"/>
+      <c r="AG226" s="2" t="n"/>
+      <c r="AH226" s="2" t="n"/>
+      <c r="AI226" s="2" t="n"/>
+      <c r="AJ226" s="2" t="n"/>
+      <c r="AK226" s="2" t="n"/>
     </row>
     <row r="227">
-      <c r="R227" t="n">
+      <c r="A227" s="2" t="n"/>
+      <c r="B227" s="2" t="n"/>
+      <c r="C227" s="2" t="n"/>
+      <c r="D227" s="2" t="n"/>
+      <c r="E227" s="2" t="n"/>
+      <c r="F227" s="2" t="n"/>
+      <c r="G227" s="2" t="n"/>
+      <c r="H227" s="2" t="n"/>
+      <c r="I227" s="2" t="n"/>
+      <c r="J227" s="2" t="n"/>
+      <c r="K227" s="2" t="n"/>
+      <c r="L227" s="2" t="n"/>
+      <c r="M227" s="2" t="n"/>
+      <c r="N227" s="2" t="n"/>
+      <c r="O227" s="2" t="n"/>
+      <c r="P227" s="2" t="n"/>
+      <c r="Q227" s="2" t="n"/>
+      <c r="R227" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="S227" t="inlineStr">
+      <c r="S227" s="2" t="inlineStr">
         <is>
           <t>Check that the descriptions are in French, as per the business mapping.</t>
         </is>
       </c>
-      <c r="T227" t="inlineStr">
+      <c r="T227" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in French, as per business mapping.</t>
         </is>
       </c>
+      <c r="U227" s="2" t="n"/>
+      <c r="V227" s="2" t="n"/>
+      <c r="W227" s="2" t="n"/>
+      <c r="X227" s="2" t="n"/>
+      <c r="Y227" s="2" t="n"/>
+      <c r="Z227" s="2" t="n"/>
+      <c r="AA227" s="2" t="n"/>
+      <c r="AB227" s="2" t="n"/>
+      <c r="AC227" s="2" t="n"/>
+      <c r="AD227" s="2" t="n"/>
+      <c r="AE227" s="2" t="n"/>
+      <c r="AF227" s="2" t="n"/>
+      <c r="AG227" s="2" t="n"/>
+      <c r="AH227" s="2" t="n"/>
+      <c r="AI227" s="2" t="n"/>
+      <c r="AJ227" s="2" t="n"/>
+      <c r="AK227" s="2" t="n"/>
     </row>
     <row r="228">
-      <c r="A228" t="inlineStr">
+      <c r="A228" s="2" t="inlineStr">
         <is>
           <t>Verify Quota Button Calculation and Display</t>
         </is>
       </c>
-      <c r="C228" t="n">
+      <c r="B228" s="2" t="n"/>
+      <c r="C228" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="D228" t="inlineStr">
+      <c r="D228" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E228" t="inlineStr">
+      <c r="E228" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F228" t="inlineStr">
+      <c r="F228" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G228" t="inlineStr">
+      <c r="G228" s="2" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="H228" t="inlineStr">
+      <c r="H228" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I228" t="inlineStr">
+      <c r="I228" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web (Full Responsive Italia/Marocco)</t>
         </is>
       </c>
-      <c r="J228" t="inlineStr">
+      <c r="J228" s="2" t="inlineStr">
         <is>
           <t>SGP Generator has provided a precompilata with multiple pronostici and their odds. Bonus multipla rules are known.</t>
         </is>
       </c>
-      <c r="K228" t="inlineStr">
+      <c r="K228" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L228" t="inlineStr">
+      <c r="L228" s="2" t="inlineStr">
         <is>
           <t>Quota Button Calculation</t>
         </is>
       </c>
-      <c r="M228" t="inlineStr">
+      <c r="M228" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N228" t="n">
-        <v>1</v>
-      </c>
-      <c r="O228" t="n">
-        <v>1</v>
-      </c>
-      <c r="P228" t="inlineStr">
+      <c r="N228" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O228" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P228" s="2" t="inlineStr">
         <is>
           <t>Precompilata data with odds and bonus multipla rules.</t>
         </is>
       </c>
-      <c r="R228" t="n">
-        <v>1</v>
-      </c>
-      <c r="S228" t="inlineStr">
+      <c r="Q228" s="2" t="n"/>
+      <c r="R228" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S228" s="2" t="inlineStr">
         <is>
           <t>Access the Carosello Dett Avv page with at least one precompilata card displayed.</t>
         </is>
       </c>
-      <c r="T228" t="inlineStr">
+      <c r="T228" s="2" t="inlineStr">
         <is>
           <t>Quota button displays the correct total quota, including any bonus multipla.</t>
         </is>
       </c>
-      <c r="U228" t="inlineStr">
+      <c r="U228" s="2" t="inlineStr">
         <is>
           <t>Italy/Morocco</t>
         </is>
       </c>
-      <c r="Y228" t="inlineStr">
+      <c r="V228" s="2" t="n"/>
+      <c r="W228" s="2" t="n"/>
+      <c r="X228" s="2" t="n"/>
+      <c r="Y228" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z228" t="inlineStr">
+      <c r="Z228" s="2" t="inlineStr">
         <is>
           <t>Covers cross-device/browser consistency for carousel skeleton.</t>
         </is>
       </c>
-      <c r="AA228" t="inlineStr">
+      <c r="AA228" s="2" t="inlineStr">
         <is>
           <t>Carosello Dett Avv – Struttura Card Precompilata</t>
         </is>
       </c>
+      <c r="AB228" s="2" t="n"/>
+      <c r="AC228" s="2" t="n"/>
+      <c r="AD228" s="2" t="n"/>
+      <c r="AE228" s="2" t="n"/>
+      <c r="AF228" s="2" t="n"/>
+      <c r="AG228" s="2" t="n"/>
+      <c r="AH228" s="2" t="n"/>
+      <c r="AI228" s="2" t="n"/>
+      <c r="AJ228" s="2" t="n"/>
+      <c r="AK228" s="2" t="n"/>
     </row>
     <row r="229">
-      <c r="R229" t="n">
+      <c r="A229" s="2" t="n"/>
+      <c r="B229" s="2" t="n"/>
+      <c r="C229" s="2" t="n"/>
+      <c r="D229" s="2" t="n"/>
+      <c r="E229" s="2" t="n"/>
+      <c r="F229" s="2" t="n"/>
+      <c r="G229" s="2" t="n"/>
+      <c r="H229" s="2" t="n"/>
+      <c r="I229" s="2" t="n"/>
+      <c r="J229" s="2" t="n"/>
+      <c r="K229" s="2" t="n"/>
+      <c r="L229" s="2" t="n"/>
+      <c r="M229" s="2" t="n"/>
+      <c r="N229" s="2" t="n"/>
+      <c r="O229" s="2" t="n"/>
+      <c r="P229" s="2" t="n"/>
+      <c r="Q229" s="2" t="n"/>
+      <c r="R229" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S229" t="inlineStr">
+      <c r="S229" s="2" t="inlineStr">
         <is>
           <t>Identify the Quota button on the precompilata card.</t>
         </is>
       </c>
-      <c r="T229" t="inlineStr">
+      <c r="T229" s="2" t="inlineStr">
         <is>
           <t>Quota button displays the correct total quota, including any bonus multipla.</t>
         </is>
       </c>
+      <c r="U229" s="2" t="n"/>
+      <c r="V229" s="2" t="n"/>
+      <c r="W229" s="2" t="n"/>
+      <c r="X229" s="2" t="n"/>
+      <c r="Y229" s="2" t="n"/>
+      <c r="Z229" s="2" t="n"/>
+      <c r="AA229" s="2" t="n"/>
+      <c r="AB229" s="2" t="n"/>
+      <c r="AC229" s="2" t="n"/>
+      <c r="AD229" s="2" t="n"/>
+      <c r="AE229" s="2" t="n"/>
+      <c r="AF229" s="2" t="n"/>
+      <c r="AG229" s="2" t="n"/>
+      <c r="AH229" s="2" t="n"/>
+      <c r="AI229" s="2" t="n"/>
+      <c r="AJ229" s="2" t="n"/>
+      <c r="AK229" s="2" t="n"/>
     </row>
     <row r="230">
-      <c r="R230" t="n">
+      <c r="A230" s="2" t="n"/>
+      <c r="B230" s="2" t="n"/>
+      <c r="C230" s="2" t="n"/>
+      <c r="D230" s="2" t="n"/>
+      <c r="E230" s="2" t="n"/>
+      <c r="F230" s="2" t="n"/>
+      <c r="G230" s="2" t="n"/>
+      <c r="H230" s="2" t="n"/>
+      <c r="I230" s="2" t="n"/>
+      <c r="J230" s="2" t="n"/>
+      <c r="K230" s="2" t="n"/>
+      <c r="L230" s="2" t="n"/>
+      <c r="M230" s="2" t="n"/>
+      <c r="N230" s="2" t="n"/>
+      <c r="O230" s="2" t="n"/>
+      <c r="P230" s="2" t="n"/>
+      <c r="Q230" s="2" t="n"/>
+      <c r="R230" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S230" t="inlineStr">
+      <c r="S230" s="2" t="inlineStr">
         <is>
           <t>Obtain the individual odds (quote) for each pronostico in the precompilata.</t>
         </is>
       </c>
-      <c r="T230" t="inlineStr">
+      <c r="T230" s="2" t="inlineStr">
         <is>
           <t>Quota button displays the correct total quota, including any bonus multipla.</t>
         </is>
       </c>
+      <c r="U230" s="2" t="n"/>
+      <c r="V230" s="2" t="n"/>
+      <c r="W230" s="2" t="n"/>
+      <c r="X230" s="2" t="n"/>
+      <c r="Y230" s="2" t="n"/>
+      <c r="Z230" s="2" t="n"/>
+      <c r="AA230" s="2" t="n"/>
+      <c r="AB230" s="2" t="n"/>
+      <c r="AC230" s="2" t="n"/>
+      <c r="AD230" s="2" t="n"/>
+      <c r="AE230" s="2" t="n"/>
+      <c r="AF230" s="2" t="n"/>
+      <c r="AG230" s="2" t="n"/>
+      <c r="AH230" s="2" t="n"/>
+      <c r="AI230" s="2" t="n"/>
+      <c r="AJ230" s="2" t="n"/>
+      <c r="AK230" s="2" t="n"/>
     </row>
     <row r="231">
-      <c r="R231" t="n">
+      <c r="A231" s="2" t="n"/>
+      <c r="B231" s="2" t="n"/>
+      <c r="C231" s="2" t="n"/>
+      <c r="D231" s="2" t="n"/>
+      <c r="E231" s="2" t="n"/>
+      <c r="F231" s="2" t="n"/>
+      <c r="G231" s="2" t="n"/>
+      <c r="H231" s="2" t="n"/>
+      <c r="I231" s="2" t="n"/>
+      <c r="J231" s="2" t="n"/>
+      <c r="K231" s="2" t="n"/>
+      <c r="L231" s="2" t="n"/>
+      <c r="M231" s="2" t="n"/>
+      <c r="N231" s="2" t="n"/>
+      <c r="O231" s="2" t="n"/>
+      <c r="P231" s="2" t="n"/>
+      <c r="Q231" s="2" t="n"/>
+      <c r="R231" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="S231" t="inlineStr">
+      <c r="S231" s="2" t="inlineStr">
         <is>
           <t>Manually calculate the expected total quota (product of all individual odds, including any applicable bonus multipla).</t>
         </is>
       </c>
-      <c r="T231" t="inlineStr">
+      <c r="T231" s="2" t="inlineStr">
         <is>
           <t>Quota button displays the correct total quota, including any bonus multipla.</t>
         </is>
       </c>
+      <c r="U231" s="2" t="n"/>
+      <c r="V231" s="2" t="n"/>
+      <c r="W231" s="2" t="n"/>
+      <c r="X231" s="2" t="n"/>
+      <c r="Y231" s="2" t="n"/>
+      <c r="Z231" s="2" t="n"/>
+      <c r="AA231" s="2" t="n"/>
+      <c r="AB231" s="2" t="n"/>
+      <c r="AC231" s="2" t="n"/>
+      <c r="AD231" s="2" t="n"/>
+      <c r="AE231" s="2" t="n"/>
+      <c r="AF231" s="2" t="n"/>
+      <c r="AG231" s="2" t="n"/>
+      <c r="AH231" s="2" t="n"/>
+      <c r="AI231" s="2" t="n"/>
+      <c r="AJ231" s="2" t="n"/>
+      <c r="AK231" s="2" t="n"/>
     </row>
     <row r="232">
-      <c r="R232" t="n">
+      <c r="A232" s="2" t="n"/>
+      <c r="B232" s="2" t="n"/>
+      <c r="C232" s="2" t="n"/>
+      <c r="D232" s="2" t="n"/>
+      <c r="E232" s="2" t="n"/>
+      <c r="F232" s="2" t="n"/>
+      <c r="G232" s="2" t="n"/>
+      <c r="H232" s="2" t="n"/>
+      <c r="I232" s="2" t="n"/>
+      <c r="J232" s="2" t="n"/>
+      <c r="K232" s="2" t="n"/>
+      <c r="L232" s="2" t="n"/>
+      <c r="M232" s="2" t="n"/>
+      <c r="N232" s="2" t="n"/>
+      <c r="O232" s="2" t="n"/>
+      <c r="P232" s="2" t="n"/>
+      <c r="Q232" s="2" t="n"/>
+      <c r="R232" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="S232" t="inlineStr">
+      <c r="S232" s="2" t="inlineStr">
         <is>
           <t>Compare the displayed quota on the button with the manually calculated value.</t>
         </is>
       </c>
-      <c r="T232" t="inlineStr">
+      <c r="T232" s="2" t="inlineStr">
         <is>
           <t>Quota button displays the correct total quota, including any bonus multipla.</t>
         </is>
       </c>
+      <c r="U232" s="2" t="n"/>
+      <c r="V232" s="2" t="n"/>
+      <c r="W232" s="2" t="n"/>
+      <c r="X232" s="2" t="n"/>
+      <c r="Y232" s="2" t="n"/>
+      <c r="Z232" s="2" t="n"/>
+      <c r="AA232" s="2" t="n"/>
+      <c r="AB232" s="2" t="n"/>
+      <c r="AC232" s="2" t="n"/>
+      <c r="AD232" s="2" t="n"/>
+      <c r="AE232" s="2" t="n"/>
+      <c r="AF232" s="2" t="n"/>
+      <c r="AG232" s="2" t="n"/>
+      <c r="AH232" s="2" t="n"/>
+      <c r="AI232" s="2" t="n"/>
+      <c r="AJ232" s="2" t="n"/>
+      <c r="AK232" s="2" t="n"/>
     </row>
     <row r="233">
-      <c r="A233" t="inlineStr">
+      <c r="A233" s="2" t="inlineStr">
         <is>
           <t>Verify Pronostico Description Rendering on Mobile Devices (iOS/Android)</t>
         </is>
       </c>
-      <c r="C233" t="n">
+      <c r="B233" s="2" t="n"/>
+      <c r="C233" s="2" t="n">
         <v>78</v>
       </c>
-      <c r="D233" t="inlineStr">
+      <c r="D233" s="2" t="inlineStr">
         <is>
           <t>Mobile IOS</t>
         </is>
       </c>
-      <c r="E233" t="inlineStr">
+      <c r="E233" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F233" t="inlineStr">
+      <c r="F233" s="2" t="inlineStr">
         <is>
           <t>Smartphone</t>
         </is>
       </c>
-      <c r="G233" t="inlineStr">
+      <c r="G233" s="2" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="H233" t="inlineStr">
+      <c r="H233" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I233" t="inlineStr">
+      <c r="I233" s="2" t="inlineStr">
         <is>
           <t>iOS 16, Safari, Full Responsive Italia</t>
         </is>
       </c>
-      <c r="J233" t="inlineStr">
+      <c r="J233" s="2" t="inlineStr">
         <is>
           <t>SGP Generator has provided at least one precompilata with pronostici. User is on the Full Responsive Italia frontend via mobile.</t>
         </is>
       </c>
-      <c r="K233" t="inlineStr">
+      <c r="K233" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L233" t="inlineStr">
+      <c r="L233" s="2" t="inlineStr">
         <is>
           <t>Pronostico Description Rendering</t>
         </is>
       </c>
-      <c r="M233" t="inlineStr">
+      <c r="M233" s="2" t="inlineStr">
         <is>
           <t>ux_ui</t>
         </is>
       </c>
-      <c r="N233" t="n">
-        <v>1</v>
-      </c>
-      <c r="O233" t="n">
-        <v>1</v>
-      </c>
-      <c r="P233" t="inlineStr">
+      <c r="N233" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O233" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P233" s="2" t="inlineStr">
         <is>
           <t>Precompilata data with mapped Italian pronostici.</t>
         </is>
       </c>
-      <c r="R233" t="n">
-        <v>1</v>
-      </c>
-      <c r="S233" t="inlineStr">
+      <c r="Q233" s="2" t="n"/>
+      <c r="R233" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S233" s="2" t="inlineStr">
         <is>
           <t>Open the Carosello Dett Avv page on a mobile device (iOS or Android) using the Full Responsive Italia frontend.</t>
         </is>
       </c>
-      <c r="T233" t="inlineStr">
+      <c r="T233" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in Italian, as per business mapping, on mobile devices.</t>
         </is>
       </c>
-      <c r="U233" t="inlineStr">
+      <c r="U233" s="2" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="Y233" t="inlineStr">
+      <c r="V233" s="2" t="n"/>
+      <c r="W233" s="2" t="n"/>
+      <c r="X233" s="2" t="n"/>
+      <c r="Y233" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z233" t="inlineStr">
+      <c r="Z233" s="2" t="inlineStr">
         <is>
           <t>Covers mobile rendering only for Italian.</t>
         </is>
       </c>
-      <c r="AA233" t="inlineStr">
+      <c r="AA233" s="2" t="inlineStr">
         <is>
           <t>Carosello Dett Avv – Struttura Card Precompilata</t>
         </is>
       </c>
+      <c r="AB233" s="2" t="n"/>
+      <c r="AC233" s="2" t="n"/>
+      <c r="AD233" s="2" t="n"/>
+      <c r="AE233" s="2" t="n"/>
+      <c r="AF233" s="2" t="n"/>
+      <c r="AG233" s="2" t="n"/>
+      <c r="AH233" s="2" t="n"/>
+      <c r="AI233" s="2" t="n"/>
+      <c r="AJ233" s="2" t="n"/>
+      <c r="AK233" s="2" t="n"/>
     </row>
     <row r="234">
-      <c r="R234" t="n">
+      <c r="A234" s="2" t="n"/>
+      <c r="B234" s="2" t="n"/>
+      <c r="C234" s="2" t="n"/>
+      <c r="D234" s="2" t="n"/>
+      <c r="E234" s="2" t="n"/>
+      <c r="F234" s="2" t="n"/>
+      <c r="G234" s="2" t="n"/>
+      <c r="H234" s="2" t="n"/>
+      <c r="I234" s="2" t="n"/>
+      <c r="J234" s="2" t="n"/>
+      <c r="K234" s="2" t="n"/>
+      <c r="L234" s="2" t="n"/>
+      <c r="M234" s="2" t="n"/>
+      <c r="N234" s="2" t="n"/>
+      <c r="O234" s="2" t="n"/>
+      <c r="P234" s="2" t="n"/>
+      <c r="Q234" s="2" t="n"/>
+      <c r="R234" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S234" t="inlineStr">
+      <c r="S234" s="2" t="inlineStr">
         <is>
           <t>Identify a precompilata card for a specific avvenimento.</t>
         </is>
       </c>
-      <c r="T234" t="inlineStr">
+      <c r="T234" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in Italian, as per business mapping, on mobile devices.</t>
         </is>
       </c>
+      <c r="U234" s="2" t="n"/>
+      <c r="V234" s="2" t="n"/>
+      <c r="W234" s="2" t="n"/>
+      <c r="X234" s="2" t="n"/>
+      <c r="Y234" s="2" t="n"/>
+      <c r="Z234" s="2" t="n"/>
+      <c r="AA234" s="2" t="n"/>
+      <c r="AB234" s="2" t="n"/>
+      <c r="AC234" s="2" t="n"/>
+      <c r="AD234" s="2" t="n"/>
+      <c r="AE234" s="2" t="n"/>
+      <c r="AF234" s="2" t="n"/>
+      <c r="AG234" s="2" t="n"/>
+      <c r="AH234" s="2" t="n"/>
+      <c r="AI234" s="2" t="n"/>
+      <c r="AJ234" s="2" t="n"/>
+      <c r="AK234" s="2" t="n"/>
     </row>
     <row r="235">
-      <c r="R235" t="n">
+      <c r="A235" s="2" t="n"/>
+      <c r="B235" s="2" t="n"/>
+      <c r="C235" s="2" t="n"/>
+      <c r="D235" s="2" t="n"/>
+      <c r="E235" s="2" t="n"/>
+      <c r="F235" s="2" t="n"/>
+      <c r="G235" s="2" t="n"/>
+      <c r="H235" s="2" t="n"/>
+      <c r="I235" s="2" t="n"/>
+      <c r="J235" s="2" t="n"/>
+      <c r="K235" s="2" t="n"/>
+      <c r="L235" s="2" t="n"/>
+      <c r="M235" s="2" t="n"/>
+      <c r="N235" s="2" t="n"/>
+      <c r="O235" s="2" t="n"/>
+      <c r="P235" s="2" t="n"/>
+      <c r="Q235" s="2" t="n"/>
+      <c r="R235" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S235" t="inlineStr">
+      <c r="S235" s="2" t="inlineStr">
         <is>
           <t>For each pronostico, verify that the description is displayed as two strings: Stringa 1 (top, bold) and Stringa 2 (below, grey).</t>
         </is>
       </c>
-      <c r="T235" t="inlineStr">
+      <c r="T235" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in Italian, as per business mapping, on mobile devices.</t>
         </is>
       </c>
+      <c r="U235" s="2" t="n"/>
+      <c r="V235" s="2" t="n"/>
+      <c r="W235" s="2" t="n"/>
+      <c r="X235" s="2" t="n"/>
+      <c r="Y235" s="2" t="n"/>
+      <c r="Z235" s="2" t="n"/>
+      <c r="AA235" s="2" t="n"/>
+      <c r="AB235" s="2" t="n"/>
+      <c r="AC235" s="2" t="n"/>
+      <c r="AD235" s="2" t="n"/>
+      <c r="AE235" s="2" t="n"/>
+      <c r="AF235" s="2" t="n"/>
+      <c r="AG235" s="2" t="n"/>
+      <c r="AH235" s="2" t="n"/>
+      <c r="AI235" s="2" t="n"/>
+      <c r="AJ235" s="2" t="n"/>
+      <c r="AK235" s="2" t="n"/>
     </row>
     <row r="236">
-      <c r="R236" t="n">
+      <c r="A236" s="2" t="n"/>
+      <c r="B236" s="2" t="n"/>
+      <c r="C236" s="2" t="n"/>
+      <c r="D236" s="2" t="n"/>
+      <c r="E236" s="2" t="n"/>
+      <c r="F236" s="2" t="n"/>
+      <c r="G236" s="2" t="n"/>
+      <c r="H236" s="2" t="n"/>
+      <c r="I236" s="2" t="n"/>
+      <c r="J236" s="2" t="n"/>
+      <c r="K236" s="2" t="n"/>
+      <c r="L236" s="2" t="n"/>
+      <c r="M236" s="2" t="n"/>
+      <c r="N236" s="2" t="n"/>
+      <c r="O236" s="2" t="n"/>
+      <c r="P236" s="2" t="n"/>
+      <c r="Q236" s="2" t="n"/>
+      <c r="R236" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="S236" t="inlineStr">
+      <c r="S236" s="2" t="inlineStr">
         <is>
           <t>Check that the descriptions are in Italian, as per the business mapping.</t>
         </is>
       </c>
-      <c r="T236" t="inlineStr">
+      <c r="T236" s="2" t="inlineStr">
         <is>
           <t>All pronostici are displayed with two strings (bold and grey), in Italian, as per business mapping, on mobile devices.</t>
         </is>
       </c>
+      <c r="U236" s="2" t="n"/>
+      <c r="V236" s="2" t="n"/>
+      <c r="W236" s="2" t="n"/>
+      <c r="X236" s="2" t="n"/>
+      <c r="Y236" s="2" t="n"/>
+      <c r="Z236" s="2" t="n"/>
+      <c r="AA236" s="2" t="n"/>
+      <c r="AB236" s="2" t="n"/>
+      <c r="AC236" s="2" t="n"/>
+      <c r="AD236" s="2" t="n"/>
+      <c r="AE236" s="2" t="n"/>
+      <c r="AF236" s="2" t="n"/>
+      <c r="AG236" s="2" t="n"/>
+      <c r="AH236" s="2" t="n"/>
+      <c r="AI236" s="2" t="n"/>
+      <c r="AJ236" s="2" t="n"/>
+      <c r="AK236" s="2" t="n"/>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr">
+      <c r="A237" s="2" t="inlineStr">
         <is>
           <t>Verify Error Handling When Pronostico Mapping is Missing</t>
         </is>
       </c>
-      <c r="C237" t="n">
+      <c r="B237" s="2" t="n"/>
+      <c r="C237" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="D237" t="inlineStr">
+      <c r="D237" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E237" t="inlineStr">
+      <c r="E237" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F237" t="inlineStr">
+      <c r="F237" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G237" t="inlineStr">
+      <c r="G237" s="2" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="H237" t="inlineStr">
+      <c r="H237" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I237" t="inlineStr">
+      <c r="I237" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web (Full Responsive Italia/Marocco)</t>
         </is>
       </c>
-      <c r="J237" t="inlineStr">
+      <c r="J237" s="2" t="inlineStr">
         <is>
           <t>SGP Generator provides a precompilata with at least one pronostico missing mapped description.</t>
         </is>
       </c>
-      <c r="K237" t="inlineStr">
+      <c r="K237" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L237" t="inlineStr">
+      <c r="L237" s="2" t="inlineStr">
         <is>
           <t>Error Handling</t>
         </is>
       </c>
-      <c r="M237" t="inlineStr">
+      <c r="M237" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N237" t="n">
-        <v>1</v>
-      </c>
-      <c r="O237" t="n">
-        <v>1</v>
-      </c>
-      <c r="P237" t="inlineStr">
+      <c r="N237" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O237" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P237" s="2" t="inlineStr">
         <is>
           <t>Precompilata data with missing pronostico mapping.</t>
         </is>
       </c>
-      <c r="R237" t="n">
-        <v>1</v>
-      </c>
-      <c r="S237" t="inlineStr">
+      <c r="Q237" s="2" t="n"/>
+      <c r="R237" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S237" s="2" t="inlineStr">
         <is>
           <t>Simulate a scenario where the SGP Generator provides a precompilata with a pronostico missing the mapped description strings.</t>
         </is>
       </c>
-      <c r="T237" t="inlineStr">
+      <c r="T237" s="2" t="inlineStr">
         <is>
           <t>Frontend gracefully handles missing pronostico mapping by displaying a placeholder or default message.</t>
         </is>
       </c>
-      <c r="U237" t="inlineStr">
+      <c r="U237" s="2" t="inlineStr">
         <is>
           <t>Italy/Morocco</t>
         </is>
       </c>
-      <c r="Y237" t="inlineStr">
+      <c r="V237" s="2" t="n"/>
+      <c r="W237" s="2" t="n"/>
+      <c r="X237" s="2" t="n"/>
+      <c r="Y237" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z237" t="inlineStr">
+      <c r="Z237" s="2" t="inlineStr">
         <is>
           <t>Covers error scenario for missing mapping.</t>
         </is>
       </c>
-      <c r="AA237" t="inlineStr">
+      <c r="AA237" s="2" t="inlineStr">
         <is>
           <t>Carosello Dett Avv – Struttura Card Precompilata</t>
         </is>
       </c>
+      <c r="AB237" s="2" t="n"/>
+      <c r="AC237" s="2" t="n"/>
+      <c r="AD237" s="2" t="n"/>
+      <c r="AE237" s="2" t="n"/>
+      <c r="AF237" s="2" t="n"/>
+      <c r="AG237" s="2" t="n"/>
+      <c r="AH237" s="2" t="n"/>
+      <c r="AI237" s="2" t="n"/>
+      <c r="AJ237" s="2" t="n"/>
+      <c r="AK237" s="2" t="n"/>
     </row>
     <row r="238">
-      <c r="R238" t="n">
+      <c r="A238" s="2" t="n"/>
+      <c r="B238" s="2" t="n"/>
+      <c r="C238" s="2" t="n"/>
+      <c r="D238" s="2" t="n"/>
+      <c r="E238" s="2" t="n"/>
+      <c r="F238" s="2" t="n"/>
+      <c r="G238" s="2" t="n"/>
+      <c r="H238" s="2" t="n"/>
+      <c r="I238" s="2" t="n"/>
+      <c r="J238" s="2" t="n"/>
+      <c r="K238" s="2" t="n"/>
+      <c r="L238" s="2" t="n"/>
+      <c r="M238" s="2" t="n"/>
+      <c r="N238" s="2" t="n"/>
+      <c r="O238" s="2" t="n"/>
+      <c r="P238" s="2" t="n"/>
+      <c r="Q238" s="2" t="n"/>
+      <c r="R238" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S238" t="inlineStr">
+      <c r="S238" s="2" t="inlineStr">
         <is>
           <t>Observe how the frontend handles the missing mapping for the pronostico.</t>
         </is>
       </c>
-      <c r="T238" t="inlineStr">
+      <c r="T238" s="2" t="inlineStr">
         <is>
           <t>Frontend gracefully handles missing pronostico mapping by displaying a placeholder or default message.</t>
         </is>
       </c>
+      <c r="U238" s="2" t="n"/>
+      <c r="V238" s="2" t="n"/>
+      <c r="W238" s="2" t="n"/>
+      <c r="X238" s="2" t="n"/>
+      <c r="Y238" s="2" t="n"/>
+      <c r="Z238" s="2" t="n"/>
+      <c r="AA238" s="2" t="n"/>
+      <c r="AB238" s="2" t="n"/>
+      <c r="AC238" s="2" t="n"/>
+      <c r="AD238" s="2" t="n"/>
+      <c r="AE238" s="2" t="n"/>
+      <c r="AF238" s="2" t="n"/>
+      <c r="AG238" s="2" t="n"/>
+      <c r="AH238" s="2" t="n"/>
+      <c r="AI238" s="2" t="n"/>
+      <c r="AJ238" s="2" t="n"/>
+      <c r="AK238" s="2" t="n"/>
     </row>
     <row r="239">
-      <c r="A239" t="inlineStr">
+      <c r="A239" s="2" t="inlineStr">
         <is>
           <t>Verify Quota Button Interaction as per Norms (par 2.1.2.1)</t>
         </is>
       </c>
-      <c r="C239" t="n">
+      <c r="B239" s="2" t="n"/>
+      <c r="C239" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="D239" t="inlineStr">
+      <c r="D239" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E239" t="inlineStr">
+      <c r="E239" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F239" t="inlineStr">
+      <c r="F239" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G239" t="inlineStr">
+      <c r="G239" s="2" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="H239" t="inlineStr">
+      <c r="H239" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I239" t="inlineStr">
+      <c r="I239" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web (Full Responsive Italia/Marocco)</t>
         </is>
       </c>
-      <c r="J239" t="inlineStr">
+      <c r="J239" s="2" t="inlineStr">
         <is>
           <t>SGP Generator has provided a precompilata with a Quota button. Interaction rules from par 2.1.2.1 are available.</t>
         </is>
       </c>
-      <c r="K239" t="inlineStr">
+      <c r="K239" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L239" t="inlineStr">
+      <c r="L239" s="2" t="inlineStr">
         <is>
           <t>Quota Button Interaction</t>
         </is>
       </c>
-      <c r="M239" t="inlineStr">
+      <c r="M239" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N239" t="n">
-        <v>1</v>
-      </c>
-      <c r="O239" t="n">
-        <v>1</v>
-      </c>
-      <c r="P239" t="inlineStr">
+      <c r="N239" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O239" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P239" s="2" t="inlineStr">
         <is>
           <t>Precompilata data with Quota button.</t>
         </is>
       </c>
-      <c r="R239" t="n">
-        <v>1</v>
-      </c>
-      <c r="S239" t="inlineStr">
+      <c r="Q239" s="2" t="n"/>
+      <c r="R239" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S239" s="2" t="inlineStr">
         <is>
           <t>Access the Carosello Dett Avv page with a precompilata card containing a Quota button.</t>
         </is>
       </c>
-      <c r="T239" t="inlineStr">
+      <c r="T239" s="2" t="inlineStr">
         <is>
           <t>Quota button interaction behaves as defined in par 2.1.2.1 without errors.</t>
         </is>
       </c>
-      <c r="U239" t="inlineStr">
+      <c r="U239" s="2" t="inlineStr">
         <is>
           <t>Italy/Morocco</t>
         </is>
       </c>
-      <c r="Y239" t="inlineStr">
+      <c r="V239" s="2" t="n"/>
+      <c r="W239" s="2" t="n"/>
+      <c r="X239" s="2" t="n"/>
+      <c r="Y239" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z239" t="inlineStr">
+      <c r="Z239" s="2" t="inlineStr">
         <is>
           <t>Covers interaction only, not calculation.</t>
         </is>
       </c>
-      <c r="AA239" t="inlineStr">
+      <c r="AA239" s="2" t="inlineStr">
         <is>
           <t>Carosello Dett Avv – Struttura Card Precompilata</t>
         </is>
       </c>
+      <c r="AB239" s="2" t="n"/>
+      <c r="AC239" s="2" t="n"/>
+      <c r="AD239" s="2" t="n"/>
+      <c r="AE239" s="2" t="n"/>
+      <c r="AF239" s="2" t="n"/>
+      <c r="AG239" s="2" t="n"/>
+      <c r="AH239" s="2" t="n"/>
+      <c r="AI239" s="2" t="n"/>
+      <c r="AJ239" s="2" t="n"/>
+      <c r="AK239" s="2" t="n"/>
     </row>
     <row r="240">
-      <c r="R240" t="n">
+      <c r="A240" s="2" t="n"/>
+      <c r="B240" s="2" t="n"/>
+      <c r="C240" s="2" t="n"/>
+      <c r="D240" s="2" t="n"/>
+      <c r="E240" s="2" t="n"/>
+      <c r="F240" s="2" t="n"/>
+      <c r="G240" s="2" t="n"/>
+      <c r="H240" s="2" t="n"/>
+      <c r="I240" s="2" t="n"/>
+      <c r="J240" s="2" t="n"/>
+      <c r="K240" s="2" t="n"/>
+      <c r="L240" s="2" t="n"/>
+      <c r="M240" s="2" t="n"/>
+      <c r="N240" s="2" t="n"/>
+      <c r="O240" s="2" t="n"/>
+      <c r="P240" s="2" t="n"/>
+      <c r="Q240" s="2" t="n"/>
+      <c r="R240" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S240" t="inlineStr">
+      <c r="S240" s="2" t="inlineStr">
         <is>
           <t>Click on the Quota button.</t>
         </is>
       </c>
-      <c r="T240" t="inlineStr">
+      <c r="T240" s="2" t="inlineStr">
         <is>
           <t>Quota button interaction behaves as defined in par 2.1.2.1 without errors.</t>
         </is>
       </c>
+      <c r="U240" s="2" t="n"/>
+      <c r="V240" s="2" t="n"/>
+      <c r="W240" s="2" t="n"/>
+      <c r="X240" s="2" t="n"/>
+      <c r="Y240" s="2" t="n"/>
+      <c r="Z240" s="2" t="n"/>
+      <c r="AA240" s="2" t="n"/>
+      <c r="AB240" s="2" t="n"/>
+      <c r="AC240" s="2" t="n"/>
+      <c r="AD240" s="2" t="n"/>
+      <c r="AE240" s="2" t="n"/>
+      <c r="AF240" s="2" t="n"/>
+      <c r="AG240" s="2" t="n"/>
+      <c r="AH240" s="2" t="n"/>
+      <c r="AI240" s="2" t="n"/>
+      <c r="AJ240" s="2" t="n"/>
+      <c r="AK240" s="2" t="n"/>
     </row>
     <row r="241">
-      <c r="R241" t="n">
+      <c r="A241" s="2" t="n"/>
+      <c r="B241" s="2" t="n"/>
+      <c r="C241" s="2" t="n"/>
+      <c r="D241" s="2" t="n"/>
+      <c r="E241" s="2" t="n"/>
+      <c r="F241" s="2" t="n"/>
+      <c r="G241" s="2" t="n"/>
+      <c r="H241" s="2" t="n"/>
+      <c r="I241" s="2" t="n"/>
+      <c r="J241" s="2" t="n"/>
+      <c r="K241" s="2" t="n"/>
+      <c r="L241" s="2" t="n"/>
+      <c r="M241" s="2" t="n"/>
+      <c r="N241" s="2" t="n"/>
+      <c r="O241" s="2" t="n"/>
+      <c r="P241" s="2" t="n"/>
+      <c r="Q241" s="2" t="n"/>
+      <c r="R241" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S241" t="inlineStr">
+      <c r="S241" s="2" t="inlineStr">
         <is>
           <t>Verify that the interaction does not cause any UI errors or unexpected behavior.</t>
         </is>
       </c>
-      <c r="T241" t="inlineStr">
+      <c r="T241" s="2" t="inlineStr">
         <is>
           <t>Quota button interaction behaves as defined in par 2.1.2.1 without errors.</t>
         </is>
       </c>
+      <c r="U241" s="2" t="n"/>
+      <c r="V241" s="2" t="n"/>
+      <c r="W241" s="2" t="n"/>
+      <c r="X241" s="2" t="n"/>
+      <c r="Y241" s="2" t="n"/>
+      <c r="Z241" s="2" t="n"/>
+      <c r="AA241" s="2" t="n"/>
+      <c r="AB241" s="2" t="n"/>
+      <c r="AC241" s="2" t="n"/>
+      <c r="AD241" s="2" t="n"/>
+      <c r="AE241" s="2" t="n"/>
+      <c r="AF241" s="2" t="n"/>
+      <c r="AG241" s="2" t="n"/>
+      <c r="AH241" s="2" t="n"/>
+      <c r="AI241" s="2" t="n"/>
+      <c r="AJ241" s="2" t="n"/>
+      <c r="AK241" s="2" t="n"/>
     </row>
     <row r="242">
-      <c r="A242" t="inlineStr">
+      <c r="A242" s="2" t="inlineStr">
         <is>
           <t>Verify caching of precompiled cards for an event within X minutes</t>
         </is>
       </c>
-      <c r="C242" t="n">
+      <c r="B242" s="2" t="n"/>
+      <c r="C242" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="D242" t="inlineStr">
+      <c r="D242" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E242" t="inlineStr">
+      <c r="E242" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F242" t="inlineStr">
+      <c r="F242" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G242" t="inlineStr">
+      <c r="G242" s="2" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="H242" t="inlineStr">
+      <c r="H242" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I242" t="inlineStr">
+      <c r="I242" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web Application</t>
         </is>
       </c>
-      <c r="J242" t="inlineStr">
+      <c r="J242" s="2" t="inlineStr">
         <is>
           <t>User is authenticated and has access to the event detail page. X (cache duration) is configured as per business requirements.</t>
         </is>
       </c>
-      <c r="K242" t="inlineStr">
+      <c r="K242" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L242" t="inlineStr">
+      <c r="L242" s="2" t="inlineStr">
         <is>
           <t>Event Detail Cache</t>
         </is>
       </c>
-      <c r="M242" t="inlineStr">
+      <c r="M242" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N242" t="n">
-        <v>1</v>
-      </c>
-      <c r="O242" t="n">
-        <v>1</v>
-      </c>
-      <c r="P242" t="inlineStr">
+      <c r="N242" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O242" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P242" s="2" t="inlineStr">
         <is>
           <t>Event A with precompiled cards available; valid user credentials.</t>
         </is>
       </c>
-      <c r="R242" t="n">
-        <v>1</v>
-      </c>
-      <c r="S242" t="inlineStr">
+      <c r="Q242" s="2" t="n"/>
+      <c r="R242" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S242" s="2" t="inlineStr">
         <is>
           <t>Navigate to the detail page of a specific event (Event A) at time T0.</t>
         </is>
       </c>
-      <c r="T242" t="inlineStr">
+      <c r="T242" s="2" t="inlineStr">
         <is>
           <t>Upon returning to the event detail page within X minutes, the user sees the same precompiled cards as at the initial visit.</t>
         </is>
       </c>
-      <c r="U242" t="inlineStr">
+      <c r="U242" s="2" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="Y242" t="inlineStr">
+      <c r="V242" s="2" t="n"/>
+      <c r="W242" s="2" t="n"/>
+      <c r="X242" s="2" t="n"/>
+      <c r="Y242" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z242" t="inlineStr">
+      <c r="Z242" s="2" t="inlineStr">
         <is>
           <t>Covers interaction only, not calculation.</t>
         </is>
       </c>
-      <c r="AA242" t="inlineStr">
+      <c r="AA242" s="2" t="inlineStr">
         <is>
           <t>Memorizzazione in cache delle precompilate su avvenimento</t>
         </is>
       </c>
+      <c r="AB242" s="2" t="n"/>
+      <c r="AC242" s="2" t="n"/>
+      <c r="AD242" s="2" t="n"/>
+      <c r="AE242" s="2" t="n"/>
+      <c r="AF242" s="2" t="n"/>
+      <c r="AG242" s="2" t="n"/>
+      <c r="AH242" s="2" t="n"/>
+      <c r="AI242" s="2" t="n"/>
+      <c r="AJ242" s="2" t="n"/>
+      <c r="AK242" s="2" t="n"/>
     </row>
     <row r="243">
-      <c r="R243" t="n">
+      <c r="A243" s="2" t="n"/>
+      <c r="B243" s="2" t="n"/>
+      <c r="C243" s="2" t="n"/>
+      <c r="D243" s="2" t="n"/>
+      <c r="E243" s="2" t="n"/>
+      <c r="F243" s="2" t="n"/>
+      <c r="G243" s="2" t="n"/>
+      <c r="H243" s="2" t="n"/>
+      <c r="I243" s="2" t="n"/>
+      <c r="J243" s="2" t="n"/>
+      <c r="K243" s="2" t="n"/>
+      <c r="L243" s="2" t="n"/>
+      <c r="M243" s="2" t="n"/>
+      <c r="N243" s="2" t="n"/>
+      <c r="O243" s="2" t="n"/>
+      <c r="P243" s="2" t="n"/>
+      <c r="Q243" s="2" t="n"/>
+      <c r="R243" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S243" t="inlineStr">
+      <c r="S243" s="2" t="inlineStr">
         <is>
           <t>Navigate away from the event detail page to another section of the site.</t>
         </is>
       </c>
-      <c r="T243" t="inlineStr">
+      <c r="T243" s="2" t="inlineStr">
         <is>
           <t>Upon returning to the event detail page within X minutes, the user sees the same precompiled cards as at the initial visit.</t>
         </is>
       </c>
+      <c r="U243" s="2" t="n"/>
+      <c r="V243" s="2" t="n"/>
+      <c r="W243" s="2" t="n"/>
+      <c r="X243" s="2" t="n"/>
+      <c r="Y243" s="2" t="n"/>
+      <c r="Z243" s="2" t="n"/>
+      <c r="AA243" s="2" t="n"/>
+      <c r="AB243" s="2" t="n"/>
+      <c r="AC243" s="2" t="n"/>
+      <c r="AD243" s="2" t="n"/>
+      <c r="AE243" s="2" t="n"/>
+      <c r="AF243" s="2" t="n"/>
+      <c r="AG243" s="2" t="n"/>
+      <c r="AH243" s="2" t="n"/>
+      <c r="AI243" s="2" t="n"/>
+      <c r="AJ243" s="2" t="n"/>
+      <c r="AK243" s="2" t="n"/>
     </row>
     <row r="244">
-      <c r="R244" t="n">
+      <c r="A244" s="2" t="n"/>
+      <c r="B244" s="2" t="n"/>
+      <c r="C244" s="2" t="n"/>
+      <c r="D244" s="2" t="n"/>
+      <c r="E244" s="2" t="n"/>
+      <c r="F244" s="2" t="n"/>
+      <c r="G244" s="2" t="n"/>
+      <c r="H244" s="2" t="n"/>
+      <c r="I244" s="2" t="n"/>
+      <c r="J244" s="2" t="n"/>
+      <c r="K244" s="2" t="n"/>
+      <c r="L244" s="2" t="n"/>
+      <c r="M244" s="2" t="n"/>
+      <c r="N244" s="2" t="n"/>
+      <c r="O244" s="2" t="n"/>
+      <c r="P244" s="2" t="n"/>
+      <c r="Q244" s="2" t="n"/>
+      <c r="R244" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S244" t="inlineStr">
+      <c r="S244" s="2" t="inlineStr">
         <is>
           <t>Return to the detail page of Event A within X minutes from T0.</t>
         </is>
       </c>
-      <c r="T244" t="inlineStr">
+      <c r="T244" s="2" t="inlineStr">
         <is>
           <t>Upon returning to the event detail page within X minutes, the user sees the same precompiled cards as at the initial visit.</t>
         </is>
       </c>
+      <c r="U244" s="2" t="n"/>
+      <c r="V244" s="2" t="n"/>
+      <c r="W244" s="2" t="n"/>
+      <c r="X244" s="2" t="n"/>
+      <c r="Y244" s="2" t="n"/>
+      <c r="Z244" s="2" t="n"/>
+      <c r="AA244" s="2" t="n"/>
+      <c r="AB244" s="2" t="n"/>
+      <c r="AC244" s="2" t="n"/>
+      <c r="AD244" s="2" t="n"/>
+      <c r="AE244" s="2" t="n"/>
+      <c r="AF244" s="2" t="n"/>
+      <c r="AG244" s="2" t="n"/>
+      <c r="AH244" s="2" t="n"/>
+      <c r="AI244" s="2" t="n"/>
+      <c r="AJ244" s="2" t="n"/>
+      <c r="AK244" s="2" t="n"/>
     </row>
     <row r="245">
-      <c r="A245" t="inlineStr">
+      <c r="A245" s="2" t="inlineStr">
         <is>
           <t>Verify cache expiration of precompiled cards after X minutes</t>
         </is>
       </c>
-      <c r="C245" t="n">
+      <c r="B245" s="2" t="n"/>
+      <c r="C245" s="2" t="n">
         <v>82</v>
       </c>
-      <c r="D245" t="inlineStr">
+      <c r="D245" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E245" t="inlineStr">
+      <c r="E245" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F245" t="inlineStr">
+      <c r="F245" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G245" t="inlineStr">
+      <c r="G245" s="2" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="H245" t="inlineStr">
+      <c r="H245" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I245" t="inlineStr">
+      <c r="I245" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web Application</t>
         </is>
       </c>
-      <c r="J245" t="inlineStr">
+      <c r="J245" s="2" t="inlineStr">
         <is>
           <t>User is authenticated and has access to the event detail page. X (cache duration) is configured as per business requirements.</t>
         </is>
       </c>
-      <c r="K245" t="inlineStr">
+      <c r="K245" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L245" t="inlineStr">
+      <c r="L245" s="2" t="inlineStr">
         <is>
           <t>Event Detail Cache</t>
         </is>
       </c>
-      <c r="M245" t="inlineStr">
+      <c r="M245" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N245" t="n">
-        <v>1</v>
-      </c>
-      <c r="O245" t="n">
-        <v>1</v>
-      </c>
-      <c r="P245" t="inlineStr">
+      <c r="N245" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O245" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P245" s="2" t="inlineStr">
         <is>
           <t>Event B with precompiled cards available; valid user credentials.</t>
         </is>
       </c>
-      <c r="R245" t="n">
-        <v>1</v>
-      </c>
-      <c r="S245" t="inlineStr">
+      <c r="Q245" s="2" t="n"/>
+      <c r="R245" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S245" s="2" t="inlineStr">
         <is>
           <t>Navigate to the detail page of a specific event (Event B) at time T0.</t>
         </is>
       </c>
-      <c r="T245" t="inlineStr">
+      <c r="T245" s="2" t="inlineStr">
         <is>
           <t>After X minutes, returning to the event detail page causes the precompiled cards to be reloaded (not served from cache).</t>
         </is>
       </c>
-      <c r="U245" t="inlineStr">
+      <c r="U245" s="2" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="Y245" t="inlineStr">
+      <c r="V245" s="2" t="n"/>
+      <c r="W245" s="2" t="n"/>
+      <c r="X245" s="2" t="n"/>
+      <c r="Y245" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z245" t="inlineStr">
+      <c r="Z245" s="2" t="inlineStr">
         <is>
           <t>Covers interaction only, not calculation.</t>
         </is>
       </c>
-      <c r="AA245" t="inlineStr">
+      <c r="AA245" s="2" t="inlineStr">
         <is>
           <t>Memorizzazione in cache delle precompilate su avvenimento</t>
         </is>
       </c>
+      <c r="AB245" s="2" t="n"/>
+      <c r="AC245" s="2" t="n"/>
+      <c r="AD245" s="2" t="n"/>
+      <c r="AE245" s="2" t="n"/>
+      <c r="AF245" s="2" t="n"/>
+      <c r="AG245" s="2" t="n"/>
+      <c r="AH245" s="2" t="n"/>
+      <c r="AI245" s="2" t="n"/>
+      <c r="AJ245" s="2" t="n"/>
+      <c r="AK245" s="2" t="n"/>
     </row>
     <row r="246">
-      <c r="R246" t="n">
+      <c r="A246" s="2" t="n"/>
+      <c r="B246" s="2" t="n"/>
+      <c r="C246" s="2" t="n"/>
+      <c r="D246" s="2" t="n"/>
+      <c r="E246" s="2" t="n"/>
+      <c r="F246" s="2" t="n"/>
+      <c r="G246" s="2" t="n"/>
+      <c r="H246" s="2" t="n"/>
+      <c r="I246" s="2" t="n"/>
+      <c r="J246" s="2" t="n"/>
+      <c r="K246" s="2" t="n"/>
+      <c r="L246" s="2" t="n"/>
+      <c r="M246" s="2" t="n"/>
+      <c r="N246" s="2" t="n"/>
+      <c r="O246" s="2" t="n"/>
+      <c r="P246" s="2" t="n"/>
+      <c r="Q246" s="2" t="n"/>
+      <c r="R246" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S246" t="inlineStr">
+      <c r="S246" s="2" t="inlineStr">
         <is>
           <t>Navigate away from the event detail page to another section of the site.</t>
         </is>
       </c>
-      <c r="T246" t="inlineStr">
+      <c r="T246" s="2" t="inlineStr">
         <is>
           <t>After X minutes, returning to the event detail page causes the precompiled cards to be reloaded (not served from cache).</t>
         </is>
       </c>
+      <c r="U246" s="2" t="n"/>
+      <c r="V246" s="2" t="n"/>
+      <c r="W246" s="2" t="n"/>
+      <c r="X246" s="2" t="n"/>
+      <c r="Y246" s="2" t="n"/>
+      <c r="Z246" s="2" t="n"/>
+      <c r="AA246" s="2" t="n"/>
+      <c r="AB246" s="2" t="n"/>
+      <c r="AC246" s="2" t="n"/>
+      <c r="AD246" s="2" t="n"/>
+      <c r="AE246" s="2" t="n"/>
+      <c r="AF246" s="2" t="n"/>
+      <c r="AG246" s="2" t="n"/>
+      <c r="AH246" s="2" t="n"/>
+      <c r="AI246" s="2" t="n"/>
+      <c r="AJ246" s="2" t="n"/>
+      <c r="AK246" s="2" t="n"/>
     </row>
     <row r="247">
-      <c r="R247" t="n">
+      <c r="A247" s="2" t="n"/>
+      <c r="B247" s="2" t="n"/>
+      <c r="C247" s="2" t="n"/>
+      <c r="D247" s="2" t="n"/>
+      <c r="E247" s="2" t="n"/>
+      <c r="F247" s="2" t="n"/>
+      <c r="G247" s="2" t="n"/>
+      <c r="H247" s="2" t="n"/>
+      <c r="I247" s="2" t="n"/>
+      <c r="J247" s="2" t="n"/>
+      <c r="K247" s="2" t="n"/>
+      <c r="L247" s="2" t="n"/>
+      <c r="M247" s="2" t="n"/>
+      <c r="N247" s="2" t="n"/>
+      <c r="O247" s="2" t="n"/>
+      <c r="P247" s="2" t="n"/>
+      <c r="Q247" s="2" t="n"/>
+      <c r="R247" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S247" t="inlineStr">
+      <c r="S247" s="2" t="inlineStr">
         <is>
           <t>Wait for more than X minutes after T0.</t>
         </is>
       </c>
-      <c r="T247" t="inlineStr">
+      <c r="T247" s="2" t="inlineStr">
         <is>
           <t>After X minutes, returning to the event detail page causes the precompiled cards to be reloaded (not served from cache).</t>
         </is>
       </c>
+      <c r="U247" s="2" t="n"/>
+      <c r="V247" s="2" t="n"/>
+      <c r="W247" s="2" t="n"/>
+      <c r="X247" s="2" t="n"/>
+      <c r="Y247" s="2" t="n"/>
+      <c r="Z247" s="2" t="n"/>
+      <c r="AA247" s="2" t="n"/>
+      <c r="AB247" s="2" t="n"/>
+      <c r="AC247" s="2" t="n"/>
+      <c r="AD247" s="2" t="n"/>
+      <c r="AE247" s="2" t="n"/>
+      <c r="AF247" s="2" t="n"/>
+      <c r="AG247" s="2" t="n"/>
+      <c r="AH247" s="2" t="n"/>
+      <c r="AI247" s="2" t="n"/>
+      <c r="AJ247" s="2" t="n"/>
+      <c r="AK247" s="2" t="n"/>
     </row>
     <row r="248">
-      <c r="R248" t="n">
+      <c r="A248" s="2" t="n"/>
+      <c r="B248" s="2" t="n"/>
+      <c r="C248" s="2" t="n"/>
+      <c r="D248" s="2" t="n"/>
+      <c r="E248" s="2" t="n"/>
+      <c r="F248" s="2" t="n"/>
+      <c r="G248" s="2" t="n"/>
+      <c r="H248" s="2" t="n"/>
+      <c r="I248" s="2" t="n"/>
+      <c r="J248" s="2" t="n"/>
+      <c r="K248" s="2" t="n"/>
+      <c r="L248" s="2" t="n"/>
+      <c r="M248" s="2" t="n"/>
+      <c r="N248" s="2" t="n"/>
+      <c r="O248" s="2" t="n"/>
+      <c r="P248" s="2" t="n"/>
+      <c r="Q248" s="2" t="n"/>
+      <c r="R248" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="S248" t="inlineStr">
+      <c r="S248" s="2" t="inlineStr">
         <is>
           <t>Return to the detail page of Event B after X minutes have passed.</t>
         </is>
       </c>
-      <c r="T248" t="inlineStr">
+      <c r="T248" s="2" t="inlineStr">
         <is>
           <t>After X minutes, returning to the event detail page causes the precompiled cards to be reloaded (not served from cache).</t>
         </is>
       </c>
+      <c r="U248" s="2" t="n"/>
+      <c r="V248" s="2" t="n"/>
+      <c r="W248" s="2" t="n"/>
+      <c r="X248" s="2" t="n"/>
+      <c r="Y248" s="2" t="n"/>
+      <c r="Z248" s="2" t="n"/>
+      <c r="AA248" s="2" t="n"/>
+      <c r="AB248" s="2" t="n"/>
+      <c r="AC248" s="2" t="n"/>
+      <c r="AD248" s="2" t="n"/>
+      <c r="AE248" s="2" t="n"/>
+      <c r="AF248" s="2" t="n"/>
+      <c r="AG248" s="2" t="n"/>
+      <c r="AH248" s="2" t="n"/>
+      <c r="AI248" s="2" t="n"/>
+      <c r="AJ248" s="2" t="n"/>
+      <c r="AK248" s="2" t="n"/>
     </row>
     <row r="249">
-      <c r="A249" t="inlineStr">
+      <c r="A249" s="2" t="inlineStr">
         <is>
           <t>Verify caching of precompiled cards is user-specific and does not leak between users</t>
         </is>
       </c>
-      <c r="C249" t="n">
+      <c r="B249" s="2" t="n"/>
+      <c r="C249" s="2" t="n">
         <v>83</v>
       </c>
-      <c r="D249" t="inlineStr">
+      <c r="D249" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E249" t="inlineStr">
+      <c r="E249" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F249" t="inlineStr">
+      <c r="F249" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G249" t="inlineStr">
+      <c r="G249" s="2" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="H249" t="inlineStr">
+      <c r="H249" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I249" t="inlineStr">
+      <c r="I249" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web Application</t>
         </is>
       </c>
-      <c r="J249" t="inlineStr">
+      <c r="J249" s="2" t="inlineStr">
         <is>
           <t>Two distinct user accounts exist. X (cache duration) is configured as per business requirements.</t>
         </is>
       </c>
-      <c r="K249" t="inlineStr">
+      <c r="K249" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L249" t="inlineStr">
+      <c r="L249" s="2" t="inlineStr">
         <is>
           <t>Event Detail Cache</t>
         </is>
       </c>
-      <c r="M249" t="inlineStr">
+      <c r="M249" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N249" t="n">
-        <v>1</v>
-      </c>
-      <c r="O249" t="n">
-        <v>1</v>
-      </c>
-      <c r="P249" t="inlineStr">
+      <c r="N249" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O249" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P249" s="2" t="inlineStr">
         <is>
           <t>Event C with precompiled cards available; credentials for User 1 and User 2.</t>
         </is>
       </c>
-      <c r="R249" t="n">
-        <v>1</v>
-      </c>
-      <c r="S249" t="inlineStr">
+      <c r="Q249" s="2" t="n"/>
+      <c r="R249" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S249" s="2" t="inlineStr">
         <is>
           <t>User 1 logs in and navigates to the detail page of Event C at time T0.</t>
         </is>
       </c>
-      <c r="T249" t="inlineStr">
+      <c r="T249" s="2" t="inlineStr">
         <is>
           <t>Precompiled cards are cached per user session; no data leakage occurs between users.</t>
         </is>
       </c>
-      <c r="U249" t="inlineStr">
+      <c r="U249" s="2" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="Y249" t="inlineStr">
+      <c r="V249" s="2" t="n"/>
+      <c r="W249" s="2" t="n"/>
+      <c r="X249" s="2" t="n"/>
+      <c r="Y249" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z249" t="inlineStr">
+      <c r="Z249" s="2" t="inlineStr">
         <is>
           <t>Does not cover cache invalidation after X minutes.</t>
         </is>
       </c>
-      <c r="AA249" t="inlineStr">
+      <c r="AA249" s="2" t="inlineStr">
         <is>
           <t>Memorizzazione in cache delle precompilate su avvenimento</t>
         </is>
       </c>
+      <c r="AB249" s="2" t="n"/>
+      <c r="AC249" s="2" t="n"/>
+      <c r="AD249" s="2" t="n"/>
+      <c r="AE249" s="2" t="n"/>
+      <c r="AF249" s="2" t="n"/>
+      <c r="AG249" s="2" t="n"/>
+      <c r="AH249" s="2" t="n"/>
+      <c r="AI249" s="2" t="n"/>
+      <c r="AJ249" s="2" t="n"/>
+      <c r="AK249" s="2" t="n"/>
     </row>
     <row r="250">
-      <c r="R250" t="n">
+      <c r="A250" s="2" t="n"/>
+      <c r="B250" s="2" t="n"/>
+      <c r="C250" s="2" t="n"/>
+      <c r="D250" s="2" t="n"/>
+      <c r="E250" s="2" t="n"/>
+      <c r="F250" s="2" t="n"/>
+      <c r="G250" s="2" t="n"/>
+      <c r="H250" s="2" t="n"/>
+      <c r="I250" s="2" t="n"/>
+      <c r="J250" s="2" t="n"/>
+      <c r="K250" s="2" t="n"/>
+      <c r="L250" s="2" t="n"/>
+      <c r="M250" s="2" t="n"/>
+      <c r="N250" s="2" t="n"/>
+      <c r="O250" s="2" t="n"/>
+      <c r="P250" s="2" t="n"/>
+      <c r="Q250" s="2" t="n"/>
+      <c r="R250" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S250" t="inlineStr">
+      <c r="S250" s="2" t="inlineStr">
         <is>
           <t>User 1 navigates away from the event detail page.</t>
         </is>
       </c>
-      <c r="T250" t="inlineStr">
+      <c r="T250" s="2" t="inlineStr">
         <is>
           <t>Precompiled cards are cached per user session; no data leakage occurs between users.</t>
         </is>
       </c>
+      <c r="U250" s="2" t="n"/>
+      <c r="V250" s="2" t="n"/>
+      <c r="W250" s="2" t="n"/>
+      <c r="X250" s="2" t="n"/>
+      <c r="Y250" s="2" t="n"/>
+      <c r="Z250" s="2" t="n"/>
+      <c r="AA250" s="2" t="n"/>
+      <c r="AB250" s="2" t="n"/>
+      <c r="AC250" s="2" t="n"/>
+      <c r="AD250" s="2" t="n"/>
+      <c r="AE250" s="2" t="n"/>
+      <c r="AF250" s="2" t="n"/>
+      <c r="AG250" s="2" t="n"/>
+      <c r="AH250" s="2" t="n"/>
+      <c r="AI250" s="2" t="n"/>
+      <c r="AJ250" s="2" t="n"/>
+      <c r="AK250" s="2" t="n"/>
     </row>
     <row r="251">
-      <c r="R251" t="n">
+      <c r="A251" s="2" t="n"/>
+      <c r="B251" s="2" t="n"/>
+      <c r="C251" s="2" t="n"/>
+      <c r="D251" s="2" t="n"/>
+      <c r="E251" s="2" t="n"/>
+      <c r="F251" s="2" t="n"/>
+      <c r="G251" s="2" t="n"/>
+      <c r="H251" s="2" t="n"/>
+      <c r="I251" s="2" t="n"/>
+      <c r="J251" s="2" t="n"/>
+      <c r="K251" s="2" t="n"/>
+      <c r="L251" s="2" t="n"/>
+      <c r="M251" s="2" t="n"/>
+      <c r="N251" s="2" t="n"/>
+      <c r="O251" s="2" t="n"/>
+      <c r="P251" s="2" t="n"/>
+      <c r="Q251" s="2" t="n"/>
+      <c r="R251" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S251" t="inlineStr">
+      <c r="S251" s="2" t="inlineStr">
         <is>
           <t>User 2 logs in (different account) and navigates to the detail page of Event C within X minutes from T0.</t>
         </is>
       </c>
-      <c r="T251" t="inlineStr">
+      <c r="T251" s="2" t="inlineStr">
         <is>
           <t>Precompiled cards are cached per user session; no data leakage occurs between users.</t>
         </is>
       </c>
+      <c r="U251" s="2" t="n"/>
+      <c r="V251" s="2" t="n"/>
+      <c r="W251" s="2" t="n"/>
+      <c r="X251" s="2" t="n"/>
+      <c r="Y251" s="2" t="n"/>
+      <c r="Z251" s="2" t="n"/>
+      <c r="AA251" s="2" t="n"/>
+      <c r="AB251" s="2" t="n"/>
+      <c r="AC251" s="2" t="n"/>
+      <c r="AD251" s="2" t="n"/>
+      <c r="AE251" s="2" t="n"/>
+      <c r="AF251" s="2" t="n"/>
+      <c r="AG251" s="2" t="n"/>
+      <c r="AH251" s="2" t="n"/>
+      <c r="AI251" s="2" t="n"/>
+      <c r="AJ251" s="2" t="n"/>
+      <c r="AK251" s="2" t="n"/>
     </row>
     <row r="252">
-      <c r="A252" t="inlineStr">
+      <c r="A252" s="2" t="inlineStr">
         <is>
           <t>Verify that navigating to a different event does not serve cached cards from another event</t>
         </is>
       </c>
-      <c r="C252" t="n">
+      <c r="B252" s="2" t="n"/>
+      <c r="C252" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="D252" t="inlineStr">
+      <c r="D252" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E252" t="inlineStr">
+      <c r="E252" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F252" t="inlineStr">
+      <c r="F252" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G252" t="inlineStr">
+      <c r="G252" s="2" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="H252" t="inlineStr">
+      <c r="H252" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I252" t="inlineStr">
+      <c r="I252" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web Application</t>
         </is>
       </c>
-      <c r="J252" t="inlineStr">
+      <c r="J252" s="2" t="inlineStr">
         <is>
           <t>User is authenticated and has access to multiple event detail pages. X (cache duration) is configured as per business requirements.</t>
         </is>
       </c>
-      <c r="K252" t="inlineStr">
+      <c r="K252" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L252" t="inlineStr">
+      <c r="L252" s="2" t="inlineStr">
         <is>
           <t>Event Detail Cache</t>
         </is>
       </c>
-      <c r="M252" t="inlineStr">
+      <c r="M252" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N252" t="n">
-        <v>1</v>
-      </c>
-      <c r="O252" t="n">
-        <v>1</v>
-      </c>
-      <c r="P252" t="inlineStr">
+      <c r="N252" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O252" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P252" s="2" t="inlineStr">
         <is>
           <t>Events D and E with precompiled cards available; valid user credentials.</t>
         </is>
       </c>
-      <c r="R252" t="n">
-        <v>1</v>
-      </c>
-      <c r="S252" t="inlineStr">
+      <c r="Q252" s="2" t="n"/>
+      <c r="R252" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S252" s="2" t="inlineStr">
         <is>
           <t>Navigate to the detail page of Event D at time T0.</t>
         </is>
       </c>
-      <c r="T252" t="inlineStr">
+      <c r="T252" s="2" t="inlineStr">
         <is>
           <t>Each event detail page displays its own precompiled cards; no cross-event cache leakage occurs.</t>
         </is>
       </c>
-      <c r="U252" t="inlineStr">
+      <c r="U252" s="2" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="Y252" t="inlineStr">
+      <c r="V252" s="2" t="n"/>
+      <c r="W252" s="2" t="n"/>
+      <c r="X252" s="2" t="n"/>
+      <c r="Y252" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z252" t="inlineStr">
+      <c r="Z252" s="2" t="inlineStr">
         <is>
           <t>Does not cover cache expiration.</t>
         </is>
       </c>
-      <c r="AA252" t="inlineStr">
+      <c r="AA252" s="2" t="inlineStr">
         <is>
           <t>Memorizzazione in cache delle precompilate su avvenimento</t>
         </is>
       </c>
+      <c r="AB252" s="2" t="n"/>
+      <c r="AC252" s="2" t="n"/>
+      <c r="AD252" s="2" t="n"/>
+      <c r="AE252" s="2" t="n"/>
+      <c r="AF252" s="2" t="n"/>
+      <c r="AG252" s="2" t="n"/>
+      <c r="AH252" s="2" t="n"/>
+      <c r="AI252" s="2" t="n"/>
+      <c r="AJ252" s="2" t="n"/>
+      <c r="AK252" s="2" t="n"/>
     </row>
     <row r="253">
-      <c r="R253" t="n">
+      <c r="A253" s="2" t="n"/>
+      <c r="B253" s="2" t="n"/>
+      <c r="C253" s="2" t="n"/>
+      <c r="D253" s="2" t="n"/>
+      <c r="E253" s="2" t="n"/>
+      <c r="F253" s="2" t="n"/>
+      <c r="G253" s="2" t="n"/>
+      <c r="H253" s="2" t="n"/>
+      <c r="I253" s="2" t="n"/>
+      <c r="J253" s="2" t="n"/>
+      <c r="K253" s="2" t="n"/>
+      <c r="L253" s="2" t="n"/>
+      <c r="M253" s="2" t="n"/>
+      <c r="N253" s="2" t="n"/>
+      <c r="O253" s="2" t="n"/>
+      <c r="P253" s="2" t="n"/>
+      <c r="Q253" s="2" t="n"/>
+      <c r="R253" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S253" t="inlineStr">
+      <c r="S253" s="2" t="inlineStr">
         <is>
           <t>Navigate away from Event D to another section of the site.</t>
         </is>
       </c>
-      <c r="T253" t="inlineStr">
+      <c r="T253" s="2" t="inlineStr">
         <is>
           <t>Each event detail page displays its own precompiled cards; no cross-event cache leakage occurs.</t>
         </is>
       </c>
+      <c r="U253" s="2" t="n"/>
+      <c r="V253" s="2" t="n"/>
+      <c r="W253" s="2" t="n"/>
+      <c r="X253" s="2" t="n"/>
+      <c r="Y253" s="2" t="n"/>
+      <c r="Z253" s="2" t="n"/>
+      <c r="AA253" s="2" t="n"/>
+      <c r="AB253" s="2" t="n"/>
+      <c r="AC253" s="2" t="n"/>
+      <c r="AD253" s="2" t="n"/>
+      <c r="AE253" s="2" t="n"/>
+      <c r="AF253" s="2" t="n"/>
+      <c r="AG253" s="2" t="n"/>
+      <c r="AH253" s="2" t="n"/>
+      <c r="AI253" s="2" t="n"/>
+      <c r="AJ253" s="2" t="n"/>
+      <c r="AK253" s="2" t="n"/>
     </row>
     <row r="254">
-      <c r="R254" t="n">
+      <c r="A254" s="2" t="n"/>
+      <c r="B254" s="2" t="n"/>
+      <c r="C254" s="2" t="n"/>
+      <c r="D254" s="2" t="n"/>
+      <c r="E254" s="2" t="n"/>
+      <c r="F254" s="2" t="n"/>
+      <c r="G254" s="2" t="n"/>
+      <c r="H254" s="2" t="n"/>
+      <c r="I254" s="2" t="n"/>
+      <c r="J254" s="2" t="n"/>
+      <c r="K254" s="2" t="n"/>
+      <c r="L254" s="2" t="n"/>
+      <c r="M254" s="2" t="n"/>
+      <c r="N254" s="2" t="n"/>
+      <c r="O254" s="2" t="n"/>
+      <c r="P254" s="2" t="n"/>
+      <c r="Q254" s="2" t="n"/>
+      <c r="R254" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="S254" t="inlineStr">
+      <c r="S254" s="2" t="inlineStr">
         <is>
           <t>Navigate to the detail page of Event E within X minutes from T0.</t>
         </is>
       </c>
-      <c r="T254" t="inlineStr">
+      <c r="T254" s="2" t="inlineStr">
         <is>
           <t>Each event detail page displays its own precompiled cards; no cross-event cache leakage occurs.</t>
         </is>
       </c>
+      <c r="U254" s="2" t="n"/>
+      <c r="V254" s="2" t="n"/>
+      <c r="W254" s="2" t="n"/>
+      <c r="X254" s="2" t="n"/>
+      <c r="Y254" s="2" t="n"/>
+      <c r="Z254" s="2" t="n"/>
+      <c r="AA254" s="2" t="n"/>
+      <c r="AB254" s="2" t="n"/>
+      <c r="AC254" s="2" t="n"/>
+      <c r="AD254" s="2" t="n"/>
+      <c r="AE254" s="2" t="n"/>
+      <c r="AF254" s="2" t="n"/>
+      <c r="AG254" s="2" t="n"/>
+      <c r="AH254" s="2" t="n"/>
+      <c r="AI254" s="2" t="n"/>
+      <c r="AJ254" s="2" t="n"/>
+      <c r="AK254" s="2" t="n"/>
     </row>
     <row r="255">
-      <c r="A255" t="inlineStr">
+      <c r="A255" s="2" t="inlineStr">
         <is>
           <t>Verify cache refresh when precompiled cards are updated during cache period</t>
         </is>
       </c>
-      <c r="C255" t="n">
+      <c r="B255" s="2" t="n"/>
+      <c r="C255" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="D255" t="inlineStr">
+      <c r="D255" s="2" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="E255" t="inlineStr">
+      <c r="E255" s="2" t="inlineStr">
         <is>
           <t>Web</t>
         </is>
       </c>
-      <c r="F255" t="inlineStr">
+      <c r="F255" s="2" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="G255" t="inlineStr">
+      <c r="G255" s="2" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="H255" t="inlineStr">
+      <c r="H255" s="2" t="inlineStr">
         <is>
           <t>UAT</t>
         </is>
       </c>
-      <c r="I255" t="inlineStr">
+      <c r="I255" s="2" t="inlineStr">
         <is>
           <t>Windows 10, Web Application</t>
         </is>
       </c>
-      <c r="J255" t="inlineStr">
+      <c r="J255" s="2" t="inlineStr">
         <is>
           <t>User is authenticated and has access to the event detail page. Ability to update precompiled cards in backend. X (cache duration) is configured as per business requirements.</t>
         </is>
       </c>
-      <c r="K255" t="inlineStr">
+      <c r="K255" s="2" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
-      <c r="L255" t="inlineStr">
+      <c r="L255" s="2" t="inlineStr">
         <is>
           <t>Event Detail Cache</t>
         </is>
       </c>
-      <c r="M255" t="inlineStr">
+      <c r="M255" s="2" t="inlineStr">
         <is>
           <t>functional</t>
         </is>
       </c>
-      <c r="N255" t="n">
-        <v>1</v>
-      </c>
-      <c r="O255" t="n">
+      <c r="N255" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O255" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P255" t="inlineStr">
+      <c r="P255" s="2" t="inlineStr">
         <is>
           <t>Event F with precompiled cards available; valid user credentials; backend access to update cards.</t>
         </is>
       </c>
-      <c r="R255" t="n">
-        <v>1</v>
-      </c>
-      <c r="S255" t="inlineStr">
+      <c r="Q255" s="2" t="n"/>
+      <c r="R255" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S255" s="2" t="inlineStr">
         <is>
           <t>Navigate to the detail page of Event F at time T0 and note the precompiled cards displayed.</t>
         </is>
       </c>
-      <c r="T255" t="inlineStr">
+      <c r="T255" s="2" t="inlineStr">
         <is>
           <t>Cached precompiled cards are shown within X minutes even if backend data changes; after X minutes, updated cards are loaded.</t>
         </is>
       </c>
-      <c r="U255" t="inlineStr">
+      <c r="U255" s="2" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="Y255" t="inlineStr">
+      <c r="V255" s="2" t="n"/>
+      <c r="W255" s="2" t="n"/>
+      <c r="X255" s="2" t="n"/>
+      <c r="Y255" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="Z255" t="inlineStr">
+      <c r="Z255" s="2" t="inlineStr">
         <is>
           <t>Covers both cache retention and expiration with backend data change.</t>
         </is>
       </c>
-      <c r="AA255" t="inlineStr">
+      <c r="AA255" s="2" t="inlineStr">
         <is>
           <t>Memorizzazione in cache delle precompilate su avvenimento</t>
         </is>
       </c>
+      <c r="AB255" s="2" t="n"/>
+      <c r="AC255" s="2" t="n"/>
+      <c r="AD255" s="2" t="n"/>
+      <c r="AE255" s="2" t="n"/>
+      <c r="AF255" s="2" t="n"/>
+      <c r="AG255" s="2" t="n"/>
+      <c r="AH255" s="2" t="n"/>
+      <c r="AI255" s="2" t="n"/>
+      <c r="AJ255" s="2" t="n"/>
+      <c r="AK255" s="2" t="n"/>
     </row>
     <row r="256">
-      <c r="R256" t="n">
+      <c r="A256" s="2" t="n"/>
+      <c r="B256" s="2" t="n"/>
+      <c r="C256" s="2" t="n"/>
+      <c r="D256" s="2" t="n"/>
+      <c r="E256" s="2" t="n"/>
+      <c r="F256" s="2" t="n"/>
+      <c r="G256" s="2" t="n"/>
+      <c r="H256" s="2" t="n"/>
+      <c r="I256" s="2" t="n"/>
+      <c r="J256" s="2" t="n"/>
+      <c r="K256" s="2" t="n"/>
+      <c r="L256" s="2" t="n"/>
+      <c r="M256" s="2" t="n"/>
+      <c r="N256" s="2" t="n"/>
+      <c r="O256" s="2" t="n"/>
+      <c r="P256" s="2" t="n"/>
+      <c r="Q256" s="2" t="n"/>
+      <c r="R256" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S256" t="inlineStr">
+      <c r="S256" s="2" t="inlineStr">
         <is>
           <t>Navigate away from the event detail page to another section of the site.</t>
         </is>
       </c>
-      <c r="T256" t="inlineStr">
+      <c r="T256" s="2" t="inlineStr">
         <is>
           <t>Cached precompiled cards are shown within X minutes even if backend data changes; after X minutes, updated cards are loaded.</t>
         </is>
       </c>
+      <c r="U256" s="2" t="n"/>
+      <c r="V256" s="2" t="n"/>
+      <c r="W256" s="2" t="n"/>
+      <c r="X256" s="2" t="n"/>
+      <c r="Y256" s="2" t="n"/>
+      <c r="Z256" s="2" t="n"/>
+      <c r="AA256" s="2" t="n"/>
+      <c r="AB256" s="2" t="n"/>
+      <c r="AC256" s="2" t="n"/>
+      <c r="AD256" s="2" t="n"/>
+      <c r="AE256" s="2" t="n"/>
+      <c r="AF256" s="2" t="n"/>
+      <c r="AG256" s="2" t="n"/>
+      <c r="AH256" s="2" t="n"/>
+      <c r="AI256" s="2" t="n"/>
+      <c r="AJ256" s="2" t="n"/>
+      <c r="AK256" s="2" t="n"/>
     </row>
     <row r="257">
       <c r="A257" s="2" t="n"/>
@@ -13110,7 +14110,7 @@
       <c r="A274" s="2" t="n"/>
       <c r="B274" s="2" t="n"/>
       <c r="C274" s="2" t="n">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D274" s="2" t="n"/>
       <c r="E274" s="2" t="n"/>

</xml_diff>